<commit_message>
fixed life cc address
</commit_message>
<xml_diff>
--- a/data/RTG_Locations.xlsx
+++ b/data/RTG_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54551\Desktop\isochrone_testing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB27717A-DE6A-4197-92A6-8E87AF360000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24060428-FF1E-4D91-8CFE-A8EF9E9C9AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE2F5E79-50BB-468F-98F2-7382D34D6FA8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Address</t>
   </si>
@@ -576,7 +576,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +677,10 @@
         <v>5</v>
       </c>
       <c r="E5" s="4">
-        <v>36.073140000000002</v>
+        <v>36.045703400000001</v>
       </c>
       <c r="F5" s="4">
-        <v>-79.834620000000001</v>
+        <v>-79.928663</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -729,9 +729,6 @@
       </c>
       <c r="B8" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
update address version unknown
</commit_message>
<xml_diff>
--- a/data/RTG_Locations.xlsx
+++ b/data/RTG_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54551\Desktop\isochrone_testing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2451D4A7-CCCD-48CB-9ED6-9FAB38F54683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF292474-3750-49B0-86AC-24F798383907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE2F5E79-50BB-468F-98F2-7382D34D6FA8}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{EE2F5E79-50BB-468F-98F2-7382D34D6FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -588,7 +588,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,14 +756,17 @@
       <c r="B9" t="s">
         <v>46</v>
       </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="4">
-        <v>36.096483499999998</v>
+        <v>36.091069099999999</v>
       </c>
       <c r="F9" s="4">
-        <v>-79.827107900000001</v>
+        <v>-79.706162500000005</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -773,9 +776,6 @@
       <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
@@ -851,10 +851,10 @@
         <v>16</v>
       </c>
       <c r="E14" s="4">
-        <v>36.096483499999998</v>
+        <v>36.059929500000003</v>
       </c>
       <c r="F14" s="4">
-        <v>-79.827107900000001</v>
+        <v>-79.715102099999996</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>